<commit_message>
feat: adiciona lógica para processar débitos de IPVA
</commit_message>
<xml_diff>
--- a/data/BASE DETRAN GOIAS.xlsx
+++ b/data/BASE DETRAN GOIAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\TI\ROBOS\ROBOS_EM_DEV\Automação Python\DukarDespachantes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7311F8A-A9CA-4934-8168-1493A46B44EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090880EA-0133-4198-A2E4-2FC6669A2E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
@@ -1623,6 +1623,7 @@
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>